<commit_message>
add:filter date in quiz and report
</commit_message>
<xml_diff>
--- a/public/input.xlsx
+++ b/public/input.xlsx
@@ -12,6 +12,7 @@
     <sheet name="_56F9DC9755BA473782653E2940F9" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Form1!$A$1:$S$6</definedName>
     <definedName function="false" hidden="false" name="_56F9DC9755BA473782653E2940F9FormId" vbProcedure="false">"Zyu7FNNMz0Klw6Y6r1JFrC2JSx6e8i1Hq06v-ZUmuHpUODNZTjJaSEVGNlo0WldQWkgyRFM5SlEyTCQlQCN0PWcu"</definedName>
     <definedName function="false" hidden="false" name="_56F9DC9755BA473782653E2940F9ResponseSheet" vbProcedure="false">"Form1"</definedName>
     <definedName function="false" hidden="false" name="_56F9DC9755BA473782653E2940F9SourceDocId" vbProcedure="false">"{4ee6f306-f7f4-4ee2-b9bb-320f5129fad6}"</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -82,6 +83,9 @@
     <t xml:space="preserve">Sum Nilai</t>
   </si>
   <si>
+    <t xml:space="preserve">Tgl Webinar</t>
+  </si>
+  <si>
     <t xml:space="preserve">anonymous</t>
   </si>
   <si>
@@ -109,10 +113,10 @@
     <t xml:space="preserve">materi menarik</t>
   </si>
   <si>
-    <t xml:space="preserve">rutin diadakan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yudhistiro Doddy Sadewo</t>
+    <t xml:space="preserve">rutin diadakan1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">028 - 07 Mei 2021</t>
   </si>
   <si>
     <t xml:space="preserve">SH - Refinery &amp; Petrochemical</t>
@@ -127,7 +131,7 @@
     <t xml:space="preserve">rifa </t>
   </si>
   <si>
-    <t xml:space="preserve">muthia</t>
+    <t xml:space="preserve">muthia2</t>
   </si>
   <si>
     <t xml:space="preserve">Harry Septiadhy </t>
@@ -145,13 +149,19 @@
     <t xml:space="preserve">rifa cakp</t>
   </si>
   <si>
-    <t xml:space="preserve">rifa manizz</t>
+    <t xml:space="preserve">rifa manizz3</t>
   </si>
   <si>
     <t xml:space="preserve">luqman keren</t>
   </si>
   <si>
-    <t xml:space="preserve">luqman cakep</t>
+    <t xml:space="preserve">luqman cakep4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">029 - 07 Mei 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">luqman cakep5</t>
   </si>
   <si>
     <t xml:space="preserve">Zyu7FNNMz0Klw6Y6r1JFrC2JSx6e8i1Hq06v-ZUmuHpUODNZTjJaSEVGNlo0WldQWkgyRFM5SlEyTCQlQCN0PWcu</t>
@@ -171,7 +181,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -194,6 +204,19 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -203,12 +226,23 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF8FAADC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF8FAADC"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -237,7 +271,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -250,6 +284,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -259,7 +301,71 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF8FAADC"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -293,19 +399,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="29.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="11" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -363,6 +470,9 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -375,40 +485,40 @@
         <v>44326.3998726852</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P2" s="1" t="n">
         <v>100</v>
@@ -418,6 +528,9 @@
       </c>
       <c r="R2" s="0" t="n">
         <v>200</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -431,40 +544,40 @@
         <v>44326.3999074074</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P3" s="1" t="n">
         <v>100</v>
@@ -474,6 +587,9 @@
       </c>
       <c r="R3" s="0" t="n">
         <v>100</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,40 +603,40 @@
         <v>44326.3999652778</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P4" s="1" t="n">
         <v>0</v>
@@ -530,6 +646,9 @@
       </c>
       <c r="R4" s="0" t="n">
         <v>100</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,40 +662,40 @@
         <v>44326.3999652778</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P5" s="1" t="n">
         <v>100</v>
@@ -587,8 +706,71 @@
       <c r="R5" s="0" t="n">
         <v>200</v>
       </c>
+      <c r="S5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>44326.6078703704</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>44326.3999652778</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:S6"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -596,8 +778,9 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
   <tableParts>
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -613,21 +796,21 @@
       <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>